<commit_message>
remove ceil to matrix
</commit_message>
<xml_diff>
--- a/eil23_data.xlsx
+++ b/eil23_data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dalmo\PycharmProjects\hybrid_algorithm_VRP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823F1F7C-FB31-4BCE-98E2-B8BA0DF34BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6584AC-DA31-4270-8CD2-B3633A9A714E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="CAPACIDADE" sheetId="2" r:id="rId2"/>
+    <sheet name="Planilha1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
@@ -96,7 +97,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,7 +117,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -138,6 +139,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -169,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -180,6 +199,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,13 +509,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AC31" sqref="C31:AC31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B1" s="1">
         <v>0</v>
       </c>
@@ -564,7 +589,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -641,7 +666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -718,7 +743,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -795,7 +820,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -872,7 +897,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -949,7 +974,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1026,7 +1051,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1103,7 +1128,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1180,7 +1205,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1257,7 +1282,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1334,7 +1359,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1411,7 +1436,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1488,7 +1513,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1565,7 +1590,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1642,7 +1667,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1719,7 +1744,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:29">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1796,7 +1821,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:29">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1873,7 +1898,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:29">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1950,7 +1975,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:29">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2027,7 +2052,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:29">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2104,7 +2129,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:29">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2181,7 +2206,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:29">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -2258,7 +2283,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:29">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -2335,7 +2360,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="25" spans="1:29">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -2412,7 +2437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:29">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C29">
         <v>19</v>
       </c>
@@ -2480,7 +2505,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:29">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C30" s="3">
         <f>VLOOKUP(C29,CAPACIDADE!$E$2:$F$24,2,FALSE)</f>
         <v>120</v>
@@ -2570,7 +2595,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="31" spans="1:29">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C31">
         <v>23</v>
       </c>
@@ -2660,9 +2685,9 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="4:6">
+    <row r="2" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2673,7 +2698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="4:6">
+    <row r="3" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
@@ -2684,7 +2709,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="4:6">
+    <row r="4" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
@@ -2695,7 +2720,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="4:6">
+    <row r="5" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D5" s="2" t="s">
         <v>3</v>
       </c>
@@ -2706,7 +2731,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="4:6">
+    <row r="6" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D6" s="2" t="s">
         <v>4</v>
       </c>
@@ -2717,7 +2742,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="7" spans="4:6">
+    <row r="7" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
@@ -2728,7 +2753,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="8" spans="4:6">
+    <row r="8" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D8" s="2" t="s">
         <v>6</v>
       </c>
@@ -2739,7 +2764,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="9" spans="4:6">
+    <row r="9" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D9" s="2" t="s">
         <v>7</v>
       </c>
@@ -2750,7 +2775,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="10" spans="4:6">
+    <row r="10" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D10" s="2" t="s">
         <v>8</v>
       </c>
@@ -2761,7 +2786,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="4:6">
+    <row r="11" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D11" s="2" t="s">
         <v>9</v>
       </c>
@@ -2772,7 +2797,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="12" spans="4:6">
+    <row r="12" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D12" s="2" t="s">
         <v>10</v>
       </c>
@@ -2783,7 +2808,7 @@
         <v>4100</v>
       </c>
     </row>
-    <row r="13" spans="4:6">
+    <row r="13" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D13" s="2" t="s">
         <v>11</v>
       </c>
@@ -2794,7 +2819,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="14" spans="4:6">
+    <row r="14" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D14" s="2" t="s">
         <v>12</v>
       </c>
@@ -2805,7 +2830,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="15" spans="4:6">
+    <row r="15" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D15" s="2" t="s">
         <v>13</v>
       </c>
@@ -2816,7 +2841,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="16" spans="4:6">
+    <row r="16" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D16" s="2" t="s">
         <v>14</v>
       </c>
@@ -2827,7 +2852,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="17" spans="4:6">
+    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D17" s="2" t="s">
         <v>15</v>
       </c>
@@ -2838,7 +2863,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="18" spans="4:6">
+    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D18" s="2" t="s">
         <v>16</v>
       </c>
@@ -2849,7 +2874,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="4:6">
+    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D19" s="2" t="s">
         <v>17</v>
       </c>
@@ -2860,7 +2885,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="20" spans="4:6">
+    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D20" s="2" t="s">
         <v>18</v>
       </c>
@@ -2871,7 +2896,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="4:6">
+    <row r="21" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D21" s="2" t="s">
         <v>19</v>
       </c>
@@ -2882,7 +2907,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="22" spans="4:6">
+    <row r="22" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D22" s="2" t="s">
         <v>20</v>
       </c>
@@ -2893,7 +2918,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="23" spans="4:6">
+    <row r="23" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D23" s="2" t="s">
         <v>21</v>
       </c>
@@ -2904,7 +2929,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="24" spans="4:6">
+    <row r="24" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D24" s="2" t="s">
         <v>22</v>
       </c>
@@ -2919,4 +2944,849 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{237DEFAC-E595-4406-8971-6703DD0C1B20}">
+  <dimension ref="C7:BH57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="BH18" sqref="BH18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>7</v>
+      </c>
+      <c r="D13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>8</v>
+      </c>
+      <c r="D14">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>9</v>
+      </c>
+      <c r="D15">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="D16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="3:60" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>11</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
+      <c r="K17">
+        <v>23</v>
+      </c>
+      <c r="L17">
+        <v>43</v>
+      </c>
+      <c r="M17">
+        <v>41</v>
+      </c>
+      <c r="N17">
+        <v>6</v>
+      </c>
+      <c r="O17">
+        <v>37</v>
+      </c>
+      <c r="P17">
+        <v>22</v>
+      </c>
+      <c r="Q17">
+        <v>45</v>
+      </c>
+      <c r="R17">
+        <v>17</v>
+      </c>
+      <c r="S17">
+        <v>5</v>
+      </c>
+      <c r="T17">
+        <v>24</v>
+      </c>
+      <c r="U17">
+        <v>12</v>
+      </c>
+      <c r="V17">
+        <v>51</v>
+      </c>
+      <c r="W17">
+        <v>42</v>
+      </c>
+      <c r="X17">
+        <v>36</v>
+      </c>
+      <c r="Y17">
+        <v>35</v>
+      </c>
+      <c r="Z17">
+        <v>33</v>
+      </c>
+      <c r="AA17">
+        <v>34</v>
+      </c>
+      <c r="AB17">
+        <v>4</v>
+      </c>
+      <c r="AC17">
+        <v>7</v>
+      </c>
+      <c r="AD17">
+        <v>47</v>
+      </c>
+      <c r="AE17">
+        <v>31</v>
+      </c>
+      <c r="AF17">
+        <v>18</v>
+      </c>
+      <c r="AG17">
+        <v>2</v>
+      </c>
+      <c r="AH17">
+        <v>38</v>
+      </c>
+      <c r="AI17">
+        <v>14</v>
+      </c>
+      <c r="AJ17">
+        <v>9</v>
+      </c>
+      <c r="AK17">
+        <v>19</v>
+      </c>
+      <c r="AL17">
+        <v>11</v>
+      </c>
+      <c r="AM17">
+        <v>49</v>
+      </c>
+      <c r="AN17">
+        <v>20</v>
+      </c>
+      <c r="AO17">
+        <v>40</v>
+      </c>
+      <c r="AP17">
+        <v>10</v>
+      </c>
+      <c r="AQ17">
+        <v>44</v>
+      </c>
+      <c r="AR17">
+        <v>8</v>
+      </c>
+      <c r="AS17">
+        <v>13</v>
+      </c>
+      <c r="AT17">
+        <v>39</v>
+      </c>
+      <c r="AU17">
+        <v>15</v>
+      </c>
+      <c r="AV17">
+        <v>3</v>
+      </c>
+      <c r="AW17">
+        <v>28</v>
+      </c>
+      <c r="AX17">
+        <v>30</v>
+      </c>
+      <c r="AY17">
+        <v>48</v>
+      </c>
+      <c r="AZ17">
+        <v>21</v>
+      </c>
+      <c r="BA17">
+        <v>32</v>
+      </c>
+      <c r="BB17">
+        <v>16</v>
+      </c>
+      <c r="BC17">
+        <v>50</v>
+      </c>
+      <c r="BD17">
+        <v>27</v>
+      </c>
+      <c r="BE17">
+        <v>46</v>
+      </c>
+      <c r="BF17">
+        <v>26</v>
+      </c>
+      <c r="BG17">
+        <v>29</v>
+      </c>
+      <c r="BH17">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="3:60" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>12</v>
+      </c>
+      <c r="D18">
+        <v>19</v>
+      </c>
+      <c r="K18" s="6">
+        <f>VLOOKUP(K17,$C$7:$D$57,2,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="L18" s="6">
+        <f t="shared" ref="L18:BH18" si="0">VLOOKUP(L17,$C$7:$D$57,2,FALSE)</f>
+        <v>13</v>
+      </c>
+      <c r="M18" s="6">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="N18" s="6">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="O18" s="6">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="P18" s="6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="Q18" s="6">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="R18" s="6">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="S18" s="6">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="T18" s="6">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="U18" s="6">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="V18" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="W18" s="8">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="X18" s="8">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="Y18" s="8">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="Z18" s="8">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="AA18" s="8">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="AB18" s="8">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="AC18" s="8">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="AD18" s="8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="AE18" s="8">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="AF18" s="4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="AG18" s="4">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="AH18" s="4">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="AI18" s="4">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="AJ18" s="4">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="AK18" s="4">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="AL18" s="4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="AM18" s="4">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="AN18" s="4">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="AO18" s="4">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="AP18" s="9">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="AQ18" s="9">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="AR18" s="9">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="AS18" s="9">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="AT18" s="9">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="AU18" s="9">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="AV18" s="9">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="AW18" s="9">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="AX18" s="9">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="AY18" s="3">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="AZ18" s="3">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="BA18" s="3">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="BB18" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="BC18" s="3">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="BD18" s="3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="BE18" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="BF18" s="3">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="BG18" s="3">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="BH18">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="3:60" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>13</v>
+      </c>
+      <c r="D19">
+        <v>29</v>
+      </c>
+      <c r="K19" s="7">
+        <f>SUM(K18:V18)</f>
+        <v>148</v>
+      </c>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7"/>
+      <c r="V19" s="7"/>
+      <c r="W19" s="7">
+        <f>SUM(W18:AE18)</f>
+        <v>160</v>
+      </c>
+      <c r="X19" s="7"/>
+      <c r="Y19" s="7"/>
+      <c r="Z19" s="7"/>
+      <c r="AA19" s="7"/>
+      <c r="AB19" s="7"/>
+      <c r="AC19" s="7"/>
+      <c r="AD19" s="7"/>
+      <c r="AE19" s="7"/>
+      <c r="AF19" s="7">
+        <f>SUM(AF18:AO18)</f>
+        <v>151</v>
+      </c>
+      <c r="AG19" s="7"/>
+      <c r="AH19" s="7"/>
+      <c r="AI19" s="7"/>
+      <c r="AJ19" s="7"/>
+      <c r="AK19" s="7"/>
+      <c r="AL19" s="7"/>
+      <c r="AM19" s="7"/>
+      <c r="AN19" s="7"/>
+      <c r="AO19" s="7"/>
+      <c r="AP19" s="7">
+        <f>SUM(AP18:AX18)</f>
+        <v>157</v>
+      </c>
+      <c r="AQ19" s="7"/>
+      <c r="AR19" s="7"/>
+      <c r="AS19" s="7"/>
+      <c r="AT19" s="7"/>
+      <c r="AU19" s="7"/>
+      <c r="AV19" s="7"/>
+      <c r="AW19" s="7"/>
+      <c r="AX19" s="7"/>
+      <c r="AY19" s="7">
+        <f>SUM(AY18:BG18)</f>
+        <v>151</v>
+      </c>
+      <c r="AZ19" s="7"/>
+      <c r="BA19" s="7"/>
+      <c r="BB19" s="7"/>
+      <c r="BC19" s="7"/>
+      <c r="BD19" s="7"/>
+      <c r="BE19" s="7"/>
+      <c r="BF19" s="7"/>
+      <c r="BG19" s="7"/>
+    </row>
+    <row r="20" spans="3:60" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>14</v>
+      </c>
+      <c r="D20">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="3:60" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>15</v>
+      </c>
+      <c r="D21">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="3:60" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>16</v>
+      </c>
+      <c r="D22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="3:60" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>17</v>
+      </c>
+      <c r="D23">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="3:60" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>18</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="3:60" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>19</v>
+      </c>
+      <c r="D25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="3:60" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>20</v>
+      </c>
+      <c r="D26">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="3:60" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>21</v>
+      </c>
+      <c r="D27">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="3:60" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>22</v>
+      </c>
+      <c r="D28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="3:60" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>23</v>
+      </c>
+      <c r="D29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="3:60" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>24</v>
+      </c>
+      <c r="D30">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="3:60" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>25</v>
+      </c>
+      <c r="D31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="3:60" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>26</v>
+      </c>
+      <c r="D32">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>27</v>
+      </c>
+      <c r="D33">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <v>28</v>
+      </c>
+      <c r="D34">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <v>29</v>
+      </c>
+      <c r="D35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <v>30</v>
+      </c>
+      <c r="D36">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <v>31</v>
+      </c>
+      <c r="D37">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <v>32</v>
+      </c>
+      <c r="D38">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <v>33</v>
+      </c>
+      <c r="D39">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <v>34</v>
+      </c>
+      <c r="D40">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <v>35</v>
+      </c>
+      <c r="D41">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <v>36</v>
+      </c>
+      <c r="D42">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <v>37</v>
+      </c>
+      <c r="D43">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C44">
+        <v>38</v>
+      </c>
+      <c r="D44">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <v>39</v>
+      </c>
+      <c r="D45">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C46">
+        <v>40</v>
+      </c>
+      <c r="D46">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C47">
+        <v>41</v>
+      </c>
+      <c r="D47">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C48">
+        <v>42</v>
+      </c>
+      <c r="D48">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C49">
+        <v>43</v>
+      </c>
+      <c r="D49">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C50">
+        <v>44</v>
+      </c>
+      <c r="D50">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C51">
+        <v>45</v>
+      </c>
+      <c r="D51">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C52">
+        <v>46</v>
+      </c>
+      <c r="D52">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C53">
+        <v>47</v>
+      </c>
+      <c r="D53">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C54">
+        <v>48</v>
+      </c>
+      <c r="D54">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C55">
+        <v>49</v>
+      </c>
+      <c r="D55">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C56">
+        <v>50</v>
+      </c>
+      <c r="D56">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C57">
+        <v>51</v>
+      </c>
+      <c r="D57">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="K19:V19"/>
+    <mergeCell ref="W19:AE19"/>
+    <mergeCell ref="AF19:AO19"/>
+    <mergeCell ref="AP19:AX19"/>
+    <mergeCell ref="AY19:BG19"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>